<commit_message>
Created fit_uv_eff and sim_model views
</commit_message>
<xml_diff>
--- a/model_sbml/test_data.xlsx
+++ b/model_sbml/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Big Chamel\Desktop\CSC3094\Psoriasis-Project\psoriasis_app\model_sbml\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\OneDrive\Desktop\csc3094\psoriasis_app\model_sbml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513BB6B5-A4BE-494A-BDCD-22512342B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D62C2-8B46-4A50-9AA7-98AE26093278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20010" yWindow="2115" windowWidth="18600" windowHeight="19350" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>LAST_FU_PASI</t>
   </si>
@@ -222,12 +219,15 @@
   <si>
     <t>UV_EFF_W_12</t>
   </si>
+  <si>
+    <t>LTFU</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -330,6 +330,11 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -355,11 +360,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -398,10 +405,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{8BFA1F5C-FDF0-44AC-BF75-C62ED5CA7F95}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{71C2F041-F5AB-4947-9CEC-8D07A5AE6764}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -783,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GC445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,35 +1218,284 @@
       <c r="FB2" s="1"/>
     </row>
     <row r="3" spans="1:185" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5"/>
-      <c r="AO3" s="5"/>
-      <c r="DR3" s="5"/>
-      <c r="FB3" s="1"/>
+      <c r="A3" s="25">
+        <v>5</v>
+      </c>
+      <c r="B3" s="24">
+        <v>14.1</v>
+      </c>
+      <c r="C3" s="24">
+        <v>12.5</v>
+      </c>
+      <c r="D3" s="24">
+        <v>6.8</v>
+      </c>
+      <c r="E3" s="24">
+        <v>6.6</v>
+      </c>
+      <c r="F3" s="24">
+        <v>3.4</v>
+      </c>
+      <c r="G3" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="H3" s="24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I3" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="J3" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="K3" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="L3" s="24">
+        <v>1.2</v>
+      </c>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="24">
+        <v>9</v>
+      </c>
+      <c r="R3" s="27">
+        <v>0.42</v>
+      </c>
+      <c r="S3" s="27">
+        <v>0.42</v>
+      </c>
+      <c r="T3" s="27">
+        <v>0.59</v>
+      </c>
+      <c r="U3" s="27">
+        <v>0.59</v>
+      </c>
+      <c r="V3" s="27">
+        <v>0.76</v>
+      </c>
+      <c r="W3" s="27">
+        <v>0.76</v>
+      </c>
+      <c r="X3" s="27">
+        <v>0.96</v>
+      </c>
+      <c r="Y3" s="27">
+        <v>0.96</v>
+      </c>
+      <c r="Z3" s="27">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AA3" s="27">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>1.32</v>
+      </c>
+      <c r="AC3" s="27">
+        <v>1.32</v>
+      </c>
+      <c r="AD3" s="27">
+        <v>1.45</v>
+      </c>
+      <c r="AE3" s="27">
+        <v>1.45</v>
+      </c>
+      <c r="AF3" s="27">
+        <v>1.52</v>
+      </c>
+      <c r="AG3" s="27">
+        <v>1.52</v>
+      </c>
+      <c r="AH3" s="27">
+        <v>1.6</v>
+      </c>
+      <c r="AI3" s="27">
+        <v>1.6</v>
+      </c>
+      <c r="AJ3" s="27">
+        <v>1.7</v>
+      </c>
+      <c r="AK3" s="27">
+        <v>1.7</v>
+      </c>
+      <c r="AL3" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="AM3" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="AN3" s="27">
+        <v>1.9</v>
+      </c>
+      <c r="AO3" s="27">
+        <v>1.9</v>
+      </c>
+      <c r="AP3" s="27">
+        <v>2</v>
+      </c>
+      <c r="AQ3" s="27">
+        <v>2</v>
+      </c>
+      <c r="AR3" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="AS3" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="AT3" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AU3" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV3" s="22"/>
+      <c r="AW3" s="22"/>
+      <c r="AX3" s="22"/>
+      <c r="AY3" s="5">
+        <f>SUM(R3:AX3)</f>
+        <v>42.940000000000012</v>
+      </c>
+      <c r="AZ3" s="22"/>
+      <c r="BA3" s="22"/>
+      <c r="BB3" s="22"/>
+      <c r="BC3" s="22"/>
+      <c r="BD3" s="22"/>
+      <c r="BE3" s="22"/>
+      <c r="BF3" s="22"/>
+      <c r="BG3" s="22"/>
+      <c r="BH3" s="22"/>
+      <c r="BI3" s="22"/>
+      <c r="BJ3" s="22"/>
+      <c r="BK3" s="22"/>
+      <c r="BL3" s="22"/>
+      <c r="BM3" s="22"/>
+      <c r="BN3" s="22"/>
+      <c r="BO3" s="22"/>
+      <c r="BP3" s="22"/>
+      <c r="BQ3" s="22"/>
+      <c r="BR3" s="22"/>
+      <c r="BS3" s="22"/>
+      <c r="BT3" s="22"/>
+      <c r="BU3" s="22"/>
+      <c r="BV3" s="22"/>
+      <c r="BW3" s="22"/>
+      <c r="BX3" s="22"/>
+      <c r="BY3" s="22"/>
+      <c r="BZ3" s="22"/>
+      <c r="CA3" s="22"/>
+      <c r="CB3" s="22"/>
+      <c r="CC3" s="22"/>
+      <c r="CD3" s="22"/>
+      <c r="CE3" s="22"/>
+      <c r="CF3" s="22"/>
+      <c r="CG3" s="22"/>
+      <c r="CH3" s="22"/>
+      <c r="CI3" s="22"/>
+      <c r="CJ3" s="22"/>
+      <c r="CK3" s="22"/>
+      <c r="CL3" s="22"/>
+      <c r="CM3" s="22"/>
+      <c r="CN3" s="22"/>
+      <c r="CO3" s="22"/>
+      <c r="CP3" s="22"/>
+      <c r="CQ3" s="22"/>
+      <c r="CR3" s="22"/>
+      <c r="CS3" s="22"/>
+      <c r="CT3" s="22"/>
+      <c r="CU3" s="22"/>
+      <c r="CV3" s="22"/>
+      <c r="CW3" s="22"/>
+      <c r="CX3" s="22"/>
+      <c r="CY3" s="22"/>
+      <c r="CZ3" s="22"/>
+      <c r="DA3" s="22"/>
+      <c r="DB3" s="22"/>
+      <c r="DC3" s="22"/>
+      <c r="DD3" s="22"/>
+      <c r="DE3" s="22"/>
+      <c r="DF3" s="22"/>
+      <c r="DG3" s="22"/>
+      <c r="DH3" s="22"/>
+      <c r="DI3" s="22"/>
+      <c r="DJ3" s="22"/>
+      <c r="DK3" s="22"/>
+      <c r="DL3" s="22"/>
+      <c r="DM3" s="22"/>
+      <c r="DN3" s="22"/>
+      <c r="DO3" s="22"/>
+      <c r="DP3" s="22"/>
+      <c r="DQ3" s="22"/>
+      <c r="DR3" s="27"/>
+      <c r="DS3" s="22"/>
+      <c r="DT3" s="22"/>
+      <c r="DU3" s="22"/>
+      <c r="DV3" s="22"/>
+      <c r="DW3" s="22"/>
+      <c r="DX3" s="22"/>
+      <c r="DY3" s="22"/>
+      <c r="DZ3" s="22"/>
+      <c r="EA3" s="22"/>
+      <c r="EB3" s="22"/>
+      <c r="EC3" s="22"/>
+      <c r="ED3" s="22"/>
+      <c r="EE3" s="22"/>
+      <c r="EF3" s="22"/>
+      <c r="EG3" s="22"/>
+      <c r="EH3" s="22"/>
+      <c r="EI3" s="22"/>
+      <c r="EJ3" s="22"/>
+      <c r="EK3" s="22"/>
+      <c r="EL3" s="22"/>
+      <c r="EM3" s="22"/>
+      <c r="EN3" s="22"/>
+      <c r="EO3" s="22"/>
+      <c r="EP3" s="22"/>
+      <c r="EQ3" s="22"/>
+      <c r="ER3" s="22"/>
+      <c r="ES3" s="22"/>
+      <c r="ET3" s="22"/>
+      <c r="EU3" s="22"/>
+      <c r="EV3" s="22"/>
+      <c r="EW3" s="22"/>
+      <c r="EX3" s="22"/>
+      <c r="EY3" s="22"/>
+      <c r="EZ3" s="22"/>
+      <c r="FA3" s="22"/>
+      <c r="FB3" s="23"/>
+      <c r="FC3" s="22"/>
+      <c r="FD3" s="22"/>
+      <c r="FE3" s="22"/>
+      <c r="FF3" s="22"/>
+      <c r="FG3" s="22"/>
+      <c r="FH3" s="22"/>
+      <c r="FI3" s="22"/>
+      <c r="FJ3" s="22"/>
+      <c r="FK3" s="22"/>
+      <c r="FL3" s="22"/>
+      <c r="FM3" s="22"/>
+      <c r="FN3" s="22"/>
+      <c r="FO3" s="22"/>
+      <c r="FP3" s="22"/>
+      <c r="FQ3" s="22"/>
+      <c r="FR3" s="22"/>
+      <c r="FS3" s="22"/>
+      <c r="FT3" s="22"/>
+      <c r="FU3" s="22"/>
+      <c r="FV3" s="22"/>
+      <c r="FW3" s="22"/>
+      <c r="FX3" s="22"/>
+      <c r="FY3" s="22"/>
+      <c r="FZ3" s="22"/>
+      <c r="GA3" s="22"/>
+      <c r="GB3" s="22"/>
+      <c r="GC3" s="22"/>
     </row>
     <row r="5" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
Updated MATLAB test scripts
</commit_message>
<xml_diff>
--- a/model_sbml/test_data.xlsx
+++ b/model_sbml/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\OneDrive\Desktop\csc3094\psoriasis_app\model_sbml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D62C2-8B46-4A50-9AA7-98AE26093278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76875948-7575-46BA-9008-3B5A0C8B9F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
-  <si>
-    <t>LAST_FU_PASI</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -73,12 +70,6 @@
   </si>
   <si>
     <t>PASI_END_WEEK_10</t>
-  </si>
-  <si>
-    <t>PASI_END_TREATMENT</t>
-  </si>
-  <si>
-    <t>LAST_FU_MONTH</t>
   </si>
   <si>
     <t>UVB_DOSE_1</t>
@@ -212,15 +203,6 @@
   </si>
   <si>
     <t>NB: UVB doses are expressed in J/cm2</t>
-  </si>
-  <si>
-    <t>UVB_DOSE_TOTAL</t>
-  </si>
-  <si>
-    <t>UV_EFF_W_12</t>
-  </si>
-  <si>
-    <t>LTFU</t>
   </si>
 </sst>
 </file>
@@ -366,7 +348,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -399,22 +381,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -802,22 +780,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GC445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="11" width="17.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="2" customWidth="1"/>
-    <col min="13" max="14" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="2" customWidth="1"/>
-    <col min="18" max="26" width="12.5703125" style="2" customWidth="1"/>
-    <col min="27" max="50" width="13.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="12.5703125" style="2" customWidth="1"/>
+    <col min="24" max="47" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.5703125" style="2" customWidth="1"/>
     <col min="51" max="51" width="15.7109375" style="2" customWidth="1"/>
     <col min="52" max="52" width="13.5703125" style="2" customWidth="1"/>
     <col min="53" max="116" width="8.7109375" style="2"/>
@@ -875,52 +854,52 @@
   <sheetData>
     <row r="1" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>14</v>
@@ -1006,30 +985,16 @@
       <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AS1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="AT1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="19"/>
       <c r="DM1" s="1"/>
       <c r="DN1" s="1"/>
       <c r="DO1" s="1"/>
@@ -1102,425 +1067,504 @@
     </row>
     <row r="2" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D2" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="R2" s="5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="S2" s="5">
+        <v>1.51</v>
+      </c>
+      <c r="T2" s="5">
+        <v>1.91</v>
+      </c>
+      <c r="U2" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="W2" s="5">
+        <v>2.87</v>
+      </c>
+      <c r="X2" s="5">
+        <v>2.87</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>3.63</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>3.63</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>3.81</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>3.81</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>4.2</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV2" s="5"/>
+      <c r="DR2" s="5"/>
+      <c r="DU2" s="7"/>
+      <c r="FB2" s="1"/>
+    </row>
+    <row r="3" spans="1:185" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>4.7</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>1.8</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G3" s="2">
         <v>2.8</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H3" s="2">
         <v>0.8</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I3" s="2">
         <v>0.8</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J3" s="2">
         <v>0.4</v>
       </c>
-      <c r="O2" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="R2" s="5">
+      <c r="O3" s="5">
         <v>0.42</v>
       </c>
-      <c r="S2" s="5">
+      <c r="P3" s="5">
         <v>0.53</v>
       </c>
-      <c r="T2" s="5">
+      <c r="Q3" s="5">
         <v>0.74</v>
       </c>
-      <c r="U2" s="5">
+      <c r="R3" s="5">
         <v>0.92</v>
       </c>
-      <c r="V2" s="5">
+      <c r="S3" s="5">
         <v>1.2</v>
       </c>
-      <c r="W2" s="5">
+      <c r="T3" s="5">
         <v>1.2</v>
       </c>
-      <c r="X2" s="5">
+      <c r="U3" s="5">
         <v>1.5</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="V3" s="5">
         <v>1.5</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="W3" s="5">
         <v>1.8</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="X3" s="5">
         <v>1.8</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="Y3" s="5">
         <v>2.0699999999999998</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="Z3" s="5">
         <v>2.0699999999999998</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AA3" s="5">
         <v>2.2799999999999998</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AB3" s="5">
         <v>2.2799999999999998</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AC3" s="5">
         <v>2.39</v>
       </c>
-      <c r="AG2" s="5">
+      <c r="AD3" s="5">
         <v>2.39</v>
       </c>
-      <c r="AH2" s="5">
+      <c r="AE3" s="5">
         <v>2.5</v>
       </c>
-      <c r="AI2" s="5">
+      <c r="AF3" s="5">
         <v>2.5</v>
       </c>
-      <c r="AJ2" s="5">
+      <c r="AG3" s="5">
         <v>2.7</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AH3" s="5">
         <v>2.7</v>
       </c>
-      <c r="AL2" s="5">
+      <c r="AI3" s="5">
         <v>3</v>
       </c>
-      <c r="AM2" s="5">
+      <c r="AJ3" s="5">
         <v>3</v>
       </c>
-      <c r="AN2" s="5">
+      <c r="AK3" s="5">
         <v>3.2</v>
       </c>
-      <c r="AO2" s="5">
+      <c r="AL3" s="5">
         <v>3.2</v>
       </c>
-      <c r="AY2" s="5">
-        <f>SUM(R2:AX2)</f>
-        <v>47.890000000000015</v>
-      </c>
-      <c r="AZ2" s="2">
-        <v>0</v>
-      </c>
-      <c r="DR2" s="5"/>
-      <c r="FB2" s="1"/>
-    </row>
-    <row r="3" spans="1:185" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="AV3" s="5"/>
+      <c r="DR3" s="5"/>
+      <c r="FB3" s="1"/>
+    </row>
+    <row r="4" spans="1:185" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>5</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B4" s="20">
         <v>14.1</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C4" s="20">
         <v>12.5</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D4" s="20">
         <v>6.8</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E4" s="20">
         <v>6.6</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F4" s="20">
         <v>3.4</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G4" s="20">
         <v>2.1</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H4" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I4" s="20">
         <v>1.8</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J4" s="20">
         <v>1.5</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K4" s="20">
         <v>1.5</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L4" s="20">
         <v>1.2</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="26">
-        <v>1.2</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="24">
-        <v>9</v>
-      </c>
-      <c r="R3" s="27">
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="23">
         <v>0.42</v>
       </c>
-      <c r="S3" s="27">
+      <c r="P4" s="23">
         <v>0.42</v>
       </c>
-      <c r="T3" s="27">
+      <c r="Q4" s="23">
         <v>0.59</v>
       </c>
-      <c r="U3" s="27">
+      <c r="R4" s="23">
         <v>0.59</v>
       </c>
-      <c r="V3" s="27">
+      <c r="S4" s="23">
         <v>0.76</v>
       </c>
-      <c r="W3" s="27">
+      <c r="T4" s="23">
         <v>0.76</v>
       </c>
-      <c r="X3" s="27">
+      <c r="U4" s="23">
         <v>0.96</v>
       </c>
-      <c r="Y3" s="27">
+      <c r="V4" s="23">
         <v>0.96</v>
       </c>
-      <c r="Z3" s="27">
+      <c r="W4" s="23">
         <v>1.1499999999999999</v>
       </c>
-      <c r="AA3" s="27">
+      <c r="X4" s="23">
         <v>1.1499999999999999</v>
       </c>
-      <c r="AB3" s="27">
+      <c r="Y4" s="23">
         <v>1.32</v>
       </c>
-      <c r="AC3" s="27">
+      <c r="Z4" s="23">
         <v>1.32</v>
       </c>
-      <c r="AD3" s="27">
+      <c r="AA4" s="23">
         <v>1.45</v>
       </c>
-      <c r="AE3" s="27">
+      <c r="AB4" s="23">
         <v>1.45</v>
       </c>
-      <c r="AF3" s="27">
+      <c r="AC4" s="23">
         <v>1.52</v>
       </c>
-      <c r="AG3" s="27">
+      <c r="AD4" s="23">
         <v>1.52</v>
       </c>
-      <c r="AH3" s="27">
+      <c r="AE4" s="23">
         <v>1.6</v>
       </c>
-      <c r="AI3" s="27">
+      <c r="AF4" s="23">
         <v>1.6</v>
       </c>
-      <c r="AJ3" s="27">
+      <c r="AG4" s="23">
         <v>1.7</v>
       </c>
-      <c r="AK3" s="27">
+      <c r="AH4" s="23">
         <v>1.7</v>
       </c>
-      <c r="AL3" s="27">
+      <c r="AI4" s="23">
         <v>1.8</v>
       </c>
-      <c r="AM3" s="27">
+      <c r="AJ4" s="23">
         <v>1.8</v>
       </c>
-      <c r="AN3" s="27">
+      <c r="AK4" s="23">
         <v>1.9</v>
       </c>
-      <c r="AO3" s="27">
+      <c r="AL4" s="23">
         <v>1.9</v>
       </c>
-      <c r="AP3" s="27">
+      <c r="AM4" s="23">
         <v>2</v>
       </c>
-      <c r="AQ3" s="27">
+      <c r="AN4" s="23">
         <v>2</v>
       </c>
-      <c r="AR3" s="27">
+      <c r="AO4" s="23">
         <v>2.1</v>
       </c>
-      <c r="AS3" s="27">
+      <c r="AP4" s="23">
         <v>2.1</v>
       </c>
-      <c r="AT3" s="27">
+      <c r="AQ4" s="23">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AU3" s="27">
+      <c r="AR4" s="23">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AV3" s="22"/>
-      <c r="AW3" s="22"/>
-      <c r="AX3" s="22"/>
-      <c r="AY3" s="5">
-        <f>SUM(R3:AX3)</f>
-        <v>42.940000000000012</v>
-      </c>
-      <c r="AZ3" s="22"/>
-      <c r="BA3" s="22"/>
-      <c r="BB3" s="22"/>
-      <c r="BC3" s="22"/>
-      <c r="BD3" s="22"/>
-      <c r="BE3" s="22"/>
-      <c r="BF3" s="22"/>
-      <c r="BG3" s="22"/>
-      <c r="BH3" s="22"/>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="22"/>
-      <c r="BK3" s="22"/>
-      <c r="BL3" s="22"/>
-      <c r="BM3" s="22"/>
-      <c r="BN3" s="22"/>
-      <c r="BO3" s="22"/>
-      <c r="BP3" s="22"/>
-      <c r="BQ3" s="22"/>
-      <c r="BR3" s="22"/>
-      <c r="BS3" s="22"/>
-      <c r="BT3" s="22"/>
-      <c r="BU3" s="22"/>
-      <c r="BV3" s="22"/>
-      <c r="BW3" s="22"/>
-      <c r="BX3" s="22"/>
-      <c r="BY3" s="22"/>
-      <c r="BZ3" s="22"/>
-      <c r="CA3" s="22"/>
-      <c r="CB3" s="22"/>
-      <c r="CC3" s="22"/>
-      <c r="CD3" s="22"/>
-      <c r="CE3" s="22"/>
-      <c r="CF3" s="22"/>
-      <c r="CG3" s="22"/>
-      <c r="CH3" s="22"/>
-      <c r="CI3" s="22"/>
-      <c r="CJ3" s="22"/>
-      <c r="CK3" s="22"/>
-      <c r="CL3" s="22"/>
-      <c r="CM3" s="22"/>
-      <c r="CN3" s="22"/>
-      <c r="CO3" s="22"/>
-      <c r="CP3" s="22"/>
-      <c r="CQ3" s="22"/>
-      <c r="CR3" s="22"/>
-      <c r="CS3" s="22"/>
-      <c r="CT3" s="22"/>
-      <c r="CU3" s="22"/>
-      <c r="CV3" s="22"/>
-      <c r="CW3" s="22"/>
-      <c r="CX3" s="22"/>
-      <c r="CY3" s="22"/>
-      <c r="CZ3" s="22"/>
-      <c r="DA3" s="22"/>
-      <c r="DB3" s="22"/>
-      <c r="DC3" s="22"/>
-      <c r="DD3" s="22"/>
-      <c r="DE3" s="22"/>
-      <c r="DF3" s="22"/>
-      <c r="DG3" s="22"/>
-      <c r="DH3" s="22"/>
-      <c r="DI3" s="22"/>
-      <c r="DJ3" s="22"/>
-      <c r="DK3" s="22"/>
-      <c r="DL3" s="22"/>
-      <c r="DM3" s="22"/>
-      <c r="DN3" s="22"/>
-      <c r="DO3" s="22"/>
-      <c r="DP3" s="22"/>
-      <c r="DQ3" s="22"/>
-      <c r="DR3" s="27"/>
-      <c r="DS3" s="22"/>
-      <c r="DT3" s="22"/>
-      <c r="DU3" s="22"/>
-      <c r="DV3" s="22"/>
-      <c r="DW3" s="22"/>
-      <c r="DX3" s="22"/>
-      <c r="DY3" s="22"/>
-      <c r="DZ3" s="22"/>
-      <c r="EA3" s="22"/>
-      <c r="EB3" s="22"/>
-      <c r="EC3" s="22"/>
-      <c r="ED3" s="22"/>
-      <c r="EE3" s="22"/>
-      <c r="EF3" s="22"/>
-      <c r="EG3" s="22"/>
-      <c r="EH3" s="22"/>
-      <c r="EI3" s="22"/>
-      <c r="EJ3" s="22"/>
-      <c r="EK3" s="22"/>
-      <c r="EL3" s="22"/>
-      <c r="EM3" s="22"/>
-      <c r="EN3" s="22"/>
-      <c r="EO3" s="22"/>
-      <c r="EP3" s="22"/>
-      <c r="EQ3" s="22"/>
-      <c r="ER3" s="22"/>
-      <c r="ES3" s="22"/>
-      <c r="ET3" s="22"/>
-      <c r="EU3" s="22"/>
-      <c r="EV3" s="22"/>
-      <c r="EW3" s="22"/>
-      <c r="EX3" s="22"/>
-      <c r="EY3" s="22"/>
-      <c r="EZ3" s="22"/>
-      <c r="FA3" s="22"/>
-      <c r="FB3" s="23"/>
-      <c r="FC3" s="22"/>
-      <c r="FD3" s="22"/>
-      <c r="FE3" s="22"/>
-      <c r="FF3" s="22"/>
-      <c r="FG3" s="22"/>
-      <c r="FH3" s="22"/>
-      <c r="FI3" s="22"/>
-      <c r="FJ3" s="22"/>
-      <c r="FK3" s="22"/>
-      <c r="FL3" s="22"/>
-      <c r="FM3" s="22"/>
-      <c r="FN3" s="22"/>
-      <c r="FO3" s="22"/>
-      <c r="FP3" s="22"/>
-      <c r="FQ3" s="22"/>
-      <c r="FR3" s="22"/>
-      <c r="FS3" s="22"/>
-      <c r="FT3" s="22"/>
-      <c r="FU3" s="22"/>
-      <c r="FV3" s="22"/>
-      <c r="FW3" s="22"/>
-      <c r="FX3" s="22"/>
-      <c r="FY3" s="22"/>
-      <c r="FZ3" s="22"/>
-      <c r="GA3" s="22"/>
-      <c r="GB3" s="22"/>
-      <c r="GC3" s="22"/>
-    </row>
-    <row r="5" spans="1:185" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="1"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="DR5" s="5"/>
-      <c r="FB5" s="1"/>
+      <c r="AS4" s="20"/>
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="20"/>
+      <c r="BA4" s="20"/>
+      <c r="BB4" s="20"/>
+      <c r="BC4" s="20"/>
+      <c r="BD4" s="20"/>
+      <c r="BE4" s="20"/>
+      <c r="BF4" s="20"/>
+      <c r="BG4" s="20"/>
+      <c r="BH4" s="20"/>
+      <c r="BI4" s="20"/>
+      <c r="BJ4" s="20"/>
+      <c r="BK4" s="20"/>
+      <c r="BL4" s="20"/>
+      <c r="BM4" s="20"/>
+      <c r="BN4" s="20"/>
+      <c r="BO4" s="20"/>
+      <c r="BP4" s="20"/>
+      <c r="BQ4" s="20"/>
+      <c r="BR4" s="20"/>
+      <c r="BS4" s="20"/>
+      <c r="BT4" s="20"/>
+      <c r="BU4" s="20"/>
+      <c r="BV4" s="20"/>
+      <c r="BW4" s="20"/>
+      <c r="BX4" s="20"/>
+      <c r="BY4" s="20"/>
+      <c r="BZ4" s="20"/>
+      <c r="CA4" s="20"/>
+      <c r="CB4" s="20"/>
+      <c r="CC4" s="20"/>
+      <c r="CD4" s="20"/>
+      <c r="CE4" s="20"/>
+      <c r="CF4" s="20"/>
+      <c r="CG4" s="20"/>
+      <c r="CH4" s="20"/>
+      <c r="CI4" s="20"/>
+      <c r="CJ4" s="20"/>
+      <c r="CK4" s="20"/>
+      <c r="CL4" s="20"/>
+      <c r="CM4" s="20"/>
+      <c r="CN4" s="20"/>
+      <c r="CO4" s="20"/>
+      <c r="CP4" s="20"/>
+      <c r="CQ4" s="20"/>
+      <c r="CR4" s="20"/>
+      <c r="CS4" s="20"/>
+      <c r="CT4" s="20"/>
+      <c r="CU4" s="20"/>
+      <c r="CV4" s="20"/>
+      <c r="CW4" s="20"/>
+      <c r="CX4" s="20"/>
+      <c r="CY4" s="20"/>
+      <c r="CZ4" s="20"/>
+      <c r="DA4" s="20"/>
+      <c r="DB4" s="20"/>
+      <c r="DC4" s="20"/>
+      <c r="DD4" s="20"/>
+      <c r="DE4" s="20"/>
+      <c r="DF4" s="20"/>
+      <c r="DG4" s="20"/>
+      <c r="DH4" s="20"/>
+      <c r="DI4" s="20"/>
+      <c r="DJ4" s="20"/>
+      <c r="DK4" s="20"/>
+      <c r="DL4" s="20"/>
+      <c r="DM4" s="20"/>
+      <c r="DN4" s="20"/>
+      <c r="DO4" s="20"/>
+      <c r="DP4" s="20"/>
+      <c r="DQ4" s="20"/>
+      <c r="DR4" s="23"/>
+      <c r="DS4" s="20"/>
+      <c r="DT4" s="20"/>
+      <c r="DU4" s="20"/>
+      <c r="DV4" s="20"/>
+      <c r="DW4" s="20"/>
+      <c r="DX4" s="20"/>
+      <c r="DY4" s="20"/>
+      <c r="DZ4" s="20"/>
+      <c r="EA4" s="20"/>
+      <c r="EB4" s="20"/>
+      <c r="EC4" s="20"/>
+      <c r="ED4" s="20"/>
+      <c r="EE4" s="20"/>
+      <c r="EF4" s="20"/>
+      <c r="EG4" s="20"/>
+      <c r="EH4" s="20"/>
+      <c r="EI4" s="20"/>
+      <c r="EJ4" s="20"/>
+      <c r="EK4" s="20"/>
+      <c r="EL4" s="20"/>
+      <c r="EM4" s="20"/>
+      <c r="EN4" s="20"/>
+      <c r="EO4" s="20"/>
+      <c r="EP4" s="20"/>
+      <c r="EQ4" s="20"/>
+      <c r="ER4" s="20"/>
+      <c r="ES4" s="20"/>
+      <c r="ET4" s="20"/>
+      <c r="EU4" s="20"/>
+      <c r="EV4" s="20"/>
+      <c r="EW4" s="20"/>
+      <c r="EX4" s="20"/>
+      <c r="EY4" s="20"/>
+      <c r="EZ4" s="20"/>
+      <c r="FA4" s="20"/>
+      <c r="FB4" s="21"/>
+      <c r="FC4" s="20"/>
+      <c r="FD4" s="20"/>
+      <c r="FE4" s="20"/>
+      <c r="FF4" s="20"/>
+      <c r="FG4" s="20"/>
+      <c r="FH4" s="20"/>
+      <c r="FI4" s="20"/>
+      <c r="FJ4" s="20"/>
+      <c r="FK4" s="20"/>
+      <c r="FL4" s="20"/>
+      <c r="FM4" s="20"/>
+      <c r="FN4" s="20"/>
+      <c r="FO4" s="20"/>
+      <c r="FP4" s="20"/>
+      <c r="FQ4" s="20"/>
+      <c r="FR4" s="20"/>
+      <c r="FS4" s="20"/>
+      <c r="FT4" s="20"/>
+      <c r="FU4" s="20"/>
+      <c r="FV4" s="20"/>
+      <c r="FW4" s="20"/>
+      <c r="FX4" s="20"/>
+      <c r="FY4" s="20"/>
+      <c r="FZ4" s="20"/>
+      <c r="GA4" s="20"/>
+      <c r="GB4" s="20"/>
+      <c r="GC4" s="20"/>
     </row>
     <row r="6" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -6709,26 +6753,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
+      <c r="A1" s="24" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
+      <c r="A2" s="25"/>
     </row>
     <row r="3" spans="1:1" ht="84" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>